<commit_message>
added description of supplementary files provided
</commit_message>
<xml_diff>
--- a/supplementary_data_files/supplementary_data_file_key.xlsx
+++ b/supplementary_data_files/supplementary_data_file_key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackson/Dropbox (MIT)/SHARED/TRAF6_Dustin/Jackson/manuscript/figures/supplement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackson/Dropbox (MIT)/work/REPOS/TRAF6_screen/supplementary_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342D8FB2-63F8-0D41-9EE2-C780B305A7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CA277F-B4AC-2047-8AF5-8957BDA84993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="520" windowWidth="38360" windowHeight="21060" xr2:uid="{000AC21F-3137-9942-8A41-EC0A3D57FFBC}"/>
+    <workbookView xWindow="38420" yWindow="500" windowWidth="38360" windowHeight="21060" xr2:uid="{000AC21F-3137-9942-8A41-EC0A3D57FFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>Supplementary data file</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>41 MD nonbinder peptide sequences</t>
+  </si>
+  <si>
+    <t>*Filtering: Nucleotide sequences were collapsed to just the motif (*********CCT***GAA*********) and then translated into amino acid sequence. Peptides which did not match the motif (xxxPxExxx) or which contained a “*” or “X” character were removed. Any sequences that didn’t have a read count of 20 or more in at least one of the read count columns were removed.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -580,6 +583,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,9 +613,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -604,23 +625,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D32A6A4-ADDF-704C-AD94-6101E3E9D989}">
-  <dimension ref="C4:F41"/>
+  <dimension ref="C4:F43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -965,7 +971,7 @@
       </c>
     </row>
     <row r="5" spans="3:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="32" t="s">
@@ -979,8 +985,8 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="30"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
@@ -989,8 +995,8 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="30"/>
-      <c r="D7" s="33"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
@@ -999,8 +1005,8 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="30"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1009,8 +1015,8 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C9" s="30"/>
-      <c r="D9" s="33"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1019,8 +1025,8 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="30"/>
-      <c r="D10" s="33"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1029,8 +1035,8 @@
       </c>
     </row>
     <row r="11" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="31"/>
-      <c r="D11" s="34"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +1045,7 @@
       </c>
     </row>
     <row r="12" spans="3:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="32" t="s">
@@ -1053,8 +1059,8 @@
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="30"/>
-      <c r="D13" s="33"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1063,8 +1069,8 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="30"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1073,8 +1079,8 @@
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C15" s="30"/>
-      <c r="D15" s="33"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1083,8 +1089,8 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C16" s="30"/>
-      <c r="D16" s="33"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="39"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1093,8 +1099,8 @@
       </c>
     </row>
     <row r="17" spans="3:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="30"/>
-      <c r="D17" s="33"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1103,8 +1109,8 @@
       </c>
     </row>
     <row r="18" spans="3:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1113,7 +1119,7 @@
       </c>
     </row>
     <row r="19" spans="3:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="32" t="s">
@@ -1127,8 +1133,8 @@
       </c>
     </row>
     <row r="20" spans="3:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="38"/>
-      <c r="D20" s="36"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="42"/>
       <c r="E20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1137,7 +1143,7 @@
       </c>
     </row>
     <row r="21" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="32" t="s">
@@ -1151,8 +1157,8 @@
       </c>
     </row>
     <row r="22" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C22" s="38"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="16" t="s">
         <v>27</v>
       </c>
@@ -1161,8 +1167,8 @@
       </c>
     </row>
     <row r="23" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C23" s="38"/>
-      <c r="D23" s="40"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="16" t="s">
         <v>4</v>
       </c>
@@ -1171,8 +1177,8 @@
       </c>
     </row>
     <row r="24" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C24" s="38"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="16" t="s">
         <v>5</v>
       </c>
@@ -1181,8 +1187,8 @@
       </c>
     </row>
     <row r="25" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C25" s="38"/>
-      <c r="D25" s="40"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="33"/>
       <c r="E25" s="16" t="s">
         <v>6</v>
       </c>
@@ -1191,8 +1197,8 @@
       </c>
     </row>
     <row r="26" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C26" s="38"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="16" t="s">
         <v>7</v>
       </c>
@@ -1201,8 +1207,8 @@
       </c>
     </row>
     <row r="27" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C27" s="38"/>
-      <c r="D27" s="40"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="16" t="s">
         <v>8</v>
       </c>
@@ -1211,8 +1217,8 @@
       </c>
     </row>
     <row r="28" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="39"/>
-      <c r="D28" s="41"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="17" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1227,7 @@
       </c>
     </row>
     <row r="29" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="29" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="32" t="s">
@@ -1235,8 +1241,8 @@
       </c>
     </row>
     <row r="30" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C30" s="38"/>
-      <c r="D30" s="40"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="16" t="s">
         <v>27</v>
       </c>
@@ -1245,8 +1251,8 @@
       </c>
     </row>
     <row r="31" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C31" s="38"/>
-      <c r="D31" s="40"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="16" t="s">
         <v>4</v>
       </c>
@@ -1255,8 +1261,8 @@
       </c>
     </row>
     <row r="32" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C32" s="38"/>
-      <c r="D32" s="40"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="16" t="s">
         <v>5</v>
       </c>
@@ -1265,8 +1271,8 @@
       </c>
     </row>
     <row r="33" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C33" s="38"/>
-      <c r="D33" s="40"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="16" t="s">
         <v>6</v>
       </c>
@@ -1275,8 +1281,8 @@
       </c>
     </row>
     <row r="34" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C34" s="38"/>
-      <c r="D34" s="40"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="16" t="s">
         <v>7</v>
       </c>
@@ -1285,8 +1291,8 @@
       </c>
     </row>
     <row r="35" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C35" s="38"/>
-      <c r="D35" s="40"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="16" t="s">
         <v>8</v>
       </c>
@@ -1295,8 +1301,8 @@
       </c>
     </row>
     <row r="36" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="38"/>
-      <c r="D36" s="42"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="18" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1311,7 @@
       </c>
     </row>
     <row r="37" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="36" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="32" t="s">
@@ -1319,8 +1325,8 @@
       </c>
     </row>
     <row r="38" spans="3:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="C38" s="30"/>
-      <c r="D38" s="33"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="39"/>
       <c r="E38" s="2" t="s">
         <v>27</v>
       </c>
@@ -1329,8 +1335,8 @@
       </c>
     </row>
     <row r="39" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="31"/>
-      <c r="D39" s="34"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="3" t="s">
         <v>31</v>
       </c>
@@ -1366,20 +1372,29 @@
         <v>35</v>
       </c>
     </row>
+    <row r="43" spans="3:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C5:C11"/>
+    <mergeCell ref="D5:D11"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="D12:D18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="C21:C28"/>
     <mergeCell ref="D21:D28"/>
     <mergeCell ref="C29:C36"/>
     <mergeCell ref="D29:D36"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="D37:D39"/>
-    <mergeCell ref="C5:C11"/>
-    <mergeCell ref="D5:D11"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="D12:D18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>